<commit_message>
hybrid  thres and opt
</commit_message>
<xml_diff>
--- a/exp/exp.xlsx
+++ b/exp/exp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>JoinMH</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +51,10 @@
   </si>
   <si>
     <t>USPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hybrid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3780,8 +3784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3808,6 +3812,9 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
       <c r="I2" t="s">
         <v>4</v>
       </c>
@@ -4009,6 +4016,18 @@
       </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
       <c r="I40" t="s">
         <v>4</v>
       </c>
@@ -4023,6 +4042,18 @@
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>1000</v>
+      </c>
+      <c r="C41">
+        <v>257</v>
+      </c>
+      <c r="D41">
+        <v>373</v>
+      </c>
+      <c r="E41">
+        <v>383</v>
+      </c>
       <c r="I41">
         <v>1000</v>
       </c>
@@ -4037,6 +4068,18 @@
       </c>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>3000</v>
+      </c>
+      <c r="C42">
+        <v>638</v>
+      </c>
+      <c r="D42">
+        <v>533</v>
+      </c>
+      <c r="E42">
+        <v>736</v>
+      </c>
       <c r="I42">
         <v>3000</v>
       </c>
@@ -4051,6 +4094,18 @@
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>10000</v>
+      </c>
+      <c r="C43">
+        <v>2683</v>
+      </c>
+      <c r="D43">
+        <v>1162</v>
+      </c>
+      <c r="E43">
+        <v>3247</v>
+      </c>
       <c r="I43">
         <v>10000</v>
       </c>
@@ -4065,6 +4120,18 @@
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>30000</v>
+      </c>
+      <c r="C44">
+        <v>18726</v>
+      </c>
+      <c r="D44">
+        <v>3231</v>
+      </c>
+      <c r="E44">
+        <v>23968</v>
+      </c>
       <c r="I44">
         <v>30000</v>
       </c>
@@ -4079,6 +4146,18 @@
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>100000</v>
+      </c>
+      <c r="C45">
+        <v>217040</v>
+      </c>
+      <c r="D45">
+        <v>15731</v>
+      </c>
+      <c r="E45">
+        <v>259537</v>
+      </c>
       <c r="I45">
         <v>100000</v>
       </c>
@@ -4093,6 +4172,9 @@
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>300000</v>
+      </c>
       <c r="I46">
         <v>300000</v>
       </c>
@@ -4107,6 +4189,9 @@
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>1000000</v>
+      </c>
       <c r="I47">
         <v>1000000</v>
       </c>

</xml_diff>

<commit_message>
write result and add it to stat
</commit_message>
<xml_diff>
--- a/exp/exp.xlsx
+++ b/exp/exp.xlsx
@@ -29583,8 +29583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J10" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="Y36" sqref="Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -30878,50 +30878,140 @@
       <c r="S34">
         <v>10000</v>
       </c>
+      <c r="T34">
+        <v>1311</v>
+      </c>
+      <c r="U34">
+        <v>1299</v>
+      </c>
+      <c r="V34">
+        <v>1299</v>
+      </c>
     </row>
     <row r="35" spans="19:22" x14ac:dyDescent="0.3">
       <c r="S35">
         <v>15848</v>
       </c>
+      <c r="T35">
+        <v>1413</v>
+      </c>
+      <c r="U35">
+        <v>1461</v>
+      </c>
+      <c r="V35">
+        <v>1587</v>
+      </c>
     </row>
     <row r="36" spans="19:22" x14ac:dyDescent="0.3">
       <c r="S36">
         <v>25118</v>
       </c>
+      <c r="T36">
+        <v>1623</v>
+      </c>
+      <c r="U36">
+        <v>1737</v>
+      </c>
+      <c r="V36">
+        <v>1880</v>
+      </c>
     </row>
     <row r="37" spans="19:22" x14ac:dyDescent="0.3">
       <c r="S37">
         <v>39810</v>
       </c>
+      <c r="T37">
+        <v>2173</v>
+      </c>
+      <c r="U37">
+        <v>2350</v>
+      </c>
+      <c r="V37">
+        <v>2514</v>
+      </c>
     </row>
     <row r="38" spans="19:22" x14ac:dyDescent="0.3">
       <c r="S38">
         <v>63095</v>
       </c>
+      <c r="T38">
+        <v>2828</v>
+      </c>
+      <c r="U38">
+        <v>2929</v>
+      </c>
+      <c r="V38">
+        <v>3327</v>
+      </c>
     </row>
     <row r="39" spans="19:22" x14ac:dyDescent="0.3">
       <c r="S39">
         <v>100000</v>
       </c>
+      <c r="T39">
+        <v>4307</v>
+      </c>
+      <c r="U39">
+        <v>4091</v>
+      </c>
+      <c r="V39">
+        <v>4788</v>
+      </c>
     </row>
     <row r="40" spans="19:22" x14ac:dyDescent="0.3">
       <c r="S40">
         <v>158489</v>
       </c>
+      <c r="T40">
+        <v>6801</v>
+      </c>
+      <c r="U40">
+        <v>6217</v>
+      </c>
+      <c r="V40">
+        <v>7046</v>
+      </c>
     </row>
     <row r="41" spans="19:22" x14ac:dyDescent="0.3">
       <c r="S41">
         <v>251188</v>
       </c>
+      <c r="T41">
+        <v>12640</v>
+      </c>
+      <c r="U41">
+        <v>9986</v>
+      </c>
+      <c r="V41">
+        <v>11244</v>
+      </c>
     </row>
     <row r="42" spans="19:22" x14ac:dyDescent="0.3">
       <c r="S42">
         <v>398107</v>
       </c>
+      <c r="T42">
+        <v>26168</v>
+      </c>
+      <c r="U42">
+        <v>17926</v>
+      </c>
+      <c r="V42">
+        <v>19565</v>
+      </c>
     </row>
     <row r="43" spans="19:22" x14ac:dyDescent="0.3">
       <c r="S43">
         <v>630957</v>
+      </c>
+      <c r="T43">
+        <v>55172</v>
+      </c>
+      <c r="U43">
+        <v>31439</v>
+      </c>
+      <c r="V43">
+        <v>42157</v>
       </c>
     </row>
     <row r="44" spans="19:22" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
equivalence comparison stat added
</commit_message>
<xml_diff>
--- a/exp/exp.xlsx
+++ b/exp/exp.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="33">
   <si>
     <t>JoinMH</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -154,6 +154,10 @@
   </si>
   <si>
     <t>JoinMH_QL (two gram 필요부분만 생성 table T/S 모두, intersection 효율적)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JoinMH</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2231,37 +2235,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.4359999999999999</c:v>
+                  <c:v>1.2989999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.595</c:v>
+                  <c:v>1.4610000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.829</c:v>
+                  <c:v>1.7370000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.488</c:v>
+                  <c:v>2.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.14</c:v>
+                  <c:v>2.9289999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.46</c:v>
+                  <c:v>4.0910000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.6680000000000001</c:v>
+                  <c:v>6.2169999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.265000000000001</c:v>
+                  <c:v>9.9860000000000007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.681999999999999</c:v>
+                  <c:v>17.925999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.107999999999997</c:v>
+                  <c:v>31.439</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>71.483000000000004</c:v>
+                  <c:v>69.656000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -29583,8 +29587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="Y36" sqref="Y36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -29599,6 +29603,9 @@
       <c r="S2" t="s">
         <v>29</v>
       </c>
+      <c r="X2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -29682,7 +29689,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1.4359999999999999</v>
+        <v>1.2989999999999999</v>
       </c>
       <c r="I4">
         <v>1711</v>
@@ -29756,7 +29763,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>1.595</v>
+        <v>1.4610000000000001</v>
       </c>
       <c r="I5">
         <v>2012</v>
@@ -29830,7 +29837,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>1.829</v>
+        <v>1.7370000000000001</v>
       </c>
       <c r="I6">
         <v>2639</v>
@@ -29904,7 +29911,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="3"/>
-        <v>2.488</v>
+        <v>2.35</v>
       </c>
       <c r="I7">
         <v>3156</v>
@@ -29978,7 +29985,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="4"/>
-        <v>3.14</v>
+        <v>2.9289999999999998</v>
       </c>
       <c r="I8">
         <v>4272</v>
@@ -30052,7 +30059,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="5"/>
-        <v>4.46</v>
+        <v>4.0910000000000002</v>
       </c>
       <c r="I9">
         <v>6023</v>
@@ -30126,7 +30133,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="6"/>
-        <v>6.6680000000000001</v>
+        <v>6.2169999999999996</v>
       </c>
       <c r="I10">
         <v>8555</v>
@@ -30200,7 +30207,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="7"/>
-        <v>10.265000000000001</v>
+        <v>9.9860000000000007</v>
       </c>
       <c r="I11">
         <v>13312</v>
@@ -30274,7 +30281,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="8"/>
-        <v>17.681999999999999</v>
+        <v>17.925999999999998</v>
       </c>
       <c r="I12">
         <v>21579</v>
@@ -30348,7 +30355,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="9"/>
-        <v>32.107999999999997</v>
+        <v>31.439</v>
       </c>
       <c r="I13">
         <v>35678</v>
@@ -30422,7 +30429,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="10"/>
-        <v>71.483000000000004</v>
+        <v>69.656000000000006</v>
       </c>
       <c r="I14">
         <v>75083</v>
@@ -30507,7 +30514,7 @@
         <v>1711</v>
       </c>
       <c r="G17">
-        <v>1436</v>
+        <v>1299</v>
       </c>
       <c r="S17" t="s">
         <v>30</v>
@@ -30530,7 +30537,7 @@
         <v>2012</v>
       </c>
       <c r="G18">
-        <v>1595</v>
+        <v>1461</v>
       </c>
       <c r="T18">
         <v>1</v>
@@ -30559,7 +30566,7 @@
         <v>2639</v>
       </c>
       <c r="G19">
-        <v>1829</v>
+        <v>1737</v>
       </c>
       <c r="S19">
         <v>10000</v>
@@ -30591,7 +30598,7 @@
         <v>3156</v>
       </c>
       <c r="G20">
-        <v>2488</v>
+        <v>2350</v>
       </c>
       <c r="S20">
         <v>15848</v>
@@ -30623,7 +30630,7 @@
         <v>4272</v>
       </c>
       <c r="G21">
-        <v>3140</v>
+        <v>2929</v>
       </c>
       <c r="S21">
         <v>25118</v>
@@ -30655,7 +30662,7 @@
         <v>6023</v>
       </c>
       <c r="G22">
-        <v>4460</v>
+        <v>4091</v>
       </c>
       <c r="S22">
         <v>39810</v>
@@ -30687,7 +30694,7 @@
         <v>8555</v>
       </c>
       <c r="G23">
-        <v>6668</v>
+        <v>6217</v>
       </c>
       <c r="S23">
         <v>63095</v>
@@ -30719,7 +30726,7 @@
         <v>13312</v>
       </c>
       <c r="G24">
-        <v>10265</v>
+        <v>9986</v>
       </c>
       <c r="S24">
         <v>100000</v>
@@ -30751,7 +30758,7 @@
         <v>21579</v>
       </c>
       <c r="G25">
-        <v>17682</v>
+        <v>17926</v>
       </c>
       <c r="S25">
         <v>158489</v>
@@ -30783,7 +30790,7 @@
         <v>35678</v>
       </c>
       <c r="G26">
-        <v>32108</v>
+        <v>31439</v>
       </c>
       <c r="S26">
         <v>251188</v>
@@ -30815,7 +30822,7 @@
         <v>75083</v>
       </c>
       <c r="G27">
-        <v>71483</v>
+        <v>69656</v>
       </c>
       <c r="S27">
         <v>398107</v>
@@ -31017,6 +31024,15 @@
     <row r="44" spans="19:22" x14ac:dyDescent="0.3">
       <c r="S44">
         <v>1000000</v>
+      </c>
+      <c r="T44">
+        <v>120033</v>
+      </c>
+      <c r="U44">
+        <v>69656</v>
+      </c>
+      <c r="V44">
+        <v>82285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debug : sample list mistakes
</commit_message>
<xml_diff>
--- a/exp/exp.xlsx
+++ b/exp/exp.xlsx
@@ -29587,8 +29587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>